<commit_message>
Change copyright on template from 2019 -> 2023
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -150,9 +150,6 @@
     <t>${table:segments.count}</t>
   </si>
   <si>
-    <t>©2019. OC Habitats.All Rights Reserved.  Data is property of OC Habitats ™ and is to only be used with express permission from an authorized board member.  If you have been forwarded this email from someone other than OC Habitats(TM), you will need to delete or call OC Habitats  (TM) at 949.697.8651 or info@ochabitats.org to request permission.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -383,6 +380,9 @@
 Some segments may not have been surveyed due to volunteer cancellation (due to illness, weather, or some other reason).
 Some segments are regularly not getting surveyed due to access issues (parking or land structures).  
 Some segments get more attention than others since we are aware the SNPL uses these segments more often or there are issues with these segments that need more regular attention. </t>
+  </si>
+  <si>
+    <t>©2023. OC Habitats.All Rights Reserved.  Data is property of OC Habitats ™ and is to only be used with express permission from an authorized board member.  If you have been forwarded this email from someone other than OC Habitats(TM), you will need to delete or call OC Habitats  (TM) at 949.697.8651 or info@ochabitats.org to request permission.</t>
   </si>
 </sst>
 </file>
@@ -1344,6 +1344,74 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1362,78 +1430,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1698,7 +1698,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q6" sqref="Q6"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1720,43 +1720,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="141" customHeight="1">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="A1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="81"/>
+      <c r="N1" s="81"/>
+      <c r="O1" s="81"/>
+      <c r="P1" s="81"/>
+      <c r="Q1" s="81"/>
+      <c r="R1" s="81"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A2" s="59"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="61"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="85"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
@@ -1815,7 +1815,7 @@
       <c r="R3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="83" t="s">
+      <c r="S3" s="73" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1826,19 +1826,19 @@
       <c r="B4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="57" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="20" t="s">
@@ -1874,89 +1874,89 @@
       <c r="R4" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="84" t="s">
+      <c r="S4" s="74" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="63"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="54"/>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
       <c r="L5" s="32"/>
       <c r="M5" s="32"/>
       <c r="N5" s="33"/>
-      <c r="O5" s="80" t="s">
+      <c r="O5" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="80"/>
-      <c r="Q5" s="80"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
       <c r="R5" s="34"/>
-      <c r="S5" s="85"/>
+      <c r="S5" s="75"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="63"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="54"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
       <c r="K6" s="35"/>
       <c r="L6" s="32"/>
       <c r="M6" s="32"/>
       <c r="N6" s="33"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="63"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="54"/>
       <c r="Q6" s="30"/>
       <c r="R6" s="36"/>
-      <c r="S6" s="86"/>
+      <c r="S6" s="76"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="73"/>
-      <c r="B7" s="77"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="63"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="54"/>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
       <c r="L7" s="32"/>
       <c r="M7" s="32"/>
       <c r="N7" s="33"/>
-      <c r="O7" s="81"/>
-      <c r="P7" s="63"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="54"/>
       <c r="Q7" s="30"/>
       <c r="R7" s="36"/>
-      <c r="S7" s="86"/>
+      <c r="S7" s="76"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="72"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="70"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
       <c r="H8" s="39"/>
       <c r="I8" s="40"/>
       <c r="J8" s="40"/>
@@ -1964,11 +1964,11 @@
       <c r="L8" s="38"/>
       <c r="M8" s="38"/>
       <c r="N8" s="37"/>
-      <c r="O8" s="82"/>
-      <c r="P8" s="79"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="69"/>
       <c r="Q8" s="39"/>
       <c r="R8" s="41"/>
-      <c r="S8" s="82"/>
+      <c r="S8" s="72"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" thickTop="1">
       <c r="A9" s="42"/>
@@ -1992,86 +1992,86 @@
       <c r="S9" s="43"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A10" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="55"/>
+      <c r="A10" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="79"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A11" s="55"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="55"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="79"/>
+      <c r="Q11" s="79"/>
+      <c r="R11" s="79"/>
+      <c r="S11" s="79"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="55"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="79"/>
+      <c r="P12" s="79"/>
+      <c r="Q12" s="79"/>
+      <c r="R12" s="79"/>
+      <c r="S12" s="79"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A13" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
+      <c r="A13" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
+      <c r="M13" s="78"/>
       <c r="N13" s="43"/>
       <c r="O13" s="43"/>
       <c r="P13" s="43"/>
@@ -2080,19 +2080,19 @@
       <c r="S13" s="43"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="78"/>
       <c r="N14" s="43"/>
       <c r="O14" s="43"/>
       <c r="P14" s="43"/>
@@ -2101,19 +2101,19 @@
       <c r="S14" s="43"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A15" s="54"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
-      <c r="M15" s="54"/>
+      <c r="A15" s="78"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="78"/>
       <c r="N15" s="43"/>
       <c r="O15" s="43"/>
       <c r="P15" s="43"/>
@@ -2122,19 +2122,19 @@
       <c r="S15" s="43"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A16" s="54"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="78"/>
+      <c r="L16" s="78"/>
+      <c r="M16" s="78"/>
       <c r="N16" s="43"/>
       <c r="O16" s="43"/>
       <c r="P16" s="43"/>
@@ -2143,19 +2143,19 @@
       <c r="S16" s="43"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A17" s="54"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="54"/>
+      <c r="A17" s="78"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="78"/>
+      <c r="L17" s="78"/>
+      <c r="M17" s="78"/>
       <c r="N17" s="43"/>
       <c r="O17" s="43"/>
       <c r="P17" s="43"/>
@@ -2164,19 +2164,19 @@
       <c r="S17" s="43"/>
     </row>
     <row r="18" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A18" s="54"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
+      <c r="A18" s="78"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="78"/>
+      <c r="M18" s="78"/>
       <c r="N18" s="43"/>
       <c r="O18" s="43"/>
       <c r="P18" s="43"/>
@@ -2185,19 +2185,19 @@
       <c r="S18" s="43"/>
     </row>
     <row r="19" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A19" s="54"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="54"/>
+      <c r="A19" s="78"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
+      <c r="M19" s="78"/>
       <c r="N19" s="43"/>
       <c r="O19" s="43"/>
       <c r="P19" s="43"/>
@@ -2206,19 +2206,19 @@
       <c r="S19" s="43"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A20" s="54"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+      <c r="M20" s="78"/>
       <c r="N20" s="43"/>
       <c r="O20" s="43"/>
       <c r="P20" s="43"/>
@@ -6069,378 +6069,378 @@
   <sheetData>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="47"/>
     </row>
     <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>43</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="49" t="s">
         <v>45</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30">
       <c r="A6" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="49" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="A7" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
       <c r="A8" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>52</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
       <c r="A9" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
       <c r="A10" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="49" t="s">
         <v>55</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
       <c r="A11" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="49" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="49" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75">
       <c r="A12" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="47"/>
     </row>
     <row r="13" spans="1:2" ht="30">
       <c r="A13" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="49" t="s">
         <v>60</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75">
       <c r="A14" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="49" t="s">
         <v>62</v>
-      </c>
-      <c r="B14" s="49" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75">
       <c r="A15" s="48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75">
       <c r="A16" s="48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75">
       <c r="A17" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="N17" s="51" t="s">
         <v>67</v>
-      </c>
-      <c r="N17" s="51" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="30">
       <c r="A18" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="N18" s="51" t="s">
         <v>70</v>
-      </c>
-      <c r="N18" s="51" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="30">
       <c r="A19" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="N19" s="51" t="s">
         <v>73</v>
-      </c>
-      <c r="N19" s="51" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75">
       <c r="A20" s="52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="47"/>
       <c r="N20" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1">
       <c r="A21" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="49" t="s">
-        <v>77</v>
-      </c>
       <c r="N21" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1">
       <c r="A22" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="49" t="s">
-        <v>79</v>
-      </c>
       <c r="N22" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1">
       <c r="A23" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="47"/>
       <c r="N23" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1">
       <c r="A24" s="46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" s="47"/>
       <c r="N24" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1">
       <c r="A25" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="49" t="s">
+      <c r="N25" s="51" t="s">
         <v>83</v>
-      </c>
-      <c r="N25" s="51" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="49" t="s">
-        <v>86</v>
-      </c>
       <c r="N26" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
       <c r="A27" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="47"/>
       <c r="N27" s="53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="47"/>
       <c r="N28" s="53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="49" t="s">
-        <v>90</v>
-      </c>
       <c r="N29" s="53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="49" t="s">
-        <v>92</v>
-      </c>
       <c r="N30" s="53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="49" t="s">
+      <c r="N31" s="53" t="s">
         <v>94</v>
-      </c>
-      <c r="N31" s="53" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="N32" s="53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="14:14" ht="15.75" customHeight="1">
       <c r="N33" s="53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="14:14" ht="15.75" customHeight="1">
       <c r="N34" s="53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="14:14" ht="15.75" customHeight="1">
       <c r="N35" s="53" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="14:14" ht="15.75" customHeight="1">
       <c r="N36" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="14:14" ht="15.75" customHeight="1">
       <c r="N37" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="14:14" ht="15.75" customHeight="1">
       <c r="N38" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="14:14" ht="15.75" customHeight="1">
       <c r="N39" s="53" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="14:14" ht="15.75" customHeight="1">
       <c r="N40" s="53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="14:14" ht="15.75" customHeight="1">
       <c r="N41" s="53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="14:14" ht="15.75" customHeight="1">
       <c r="N42" s="53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="14:14" ht="15.75" customHeight="1">
       <c r="N43" s="53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="14:14" ht="15.75" customHeight="1">
       <c r="N44" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="14:14" ht="15.75" customHeight="1">
       <c r="N45" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="14:14" ht="15.75" customHeight="1">
       <c r="N46" s="53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="14:14" ht="15.75" customHeight="1">
       <c r="N47" s="53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="14:14" ht="15.75" customHeight="1">
       <c r="N48" s="53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="14:14" ht="15.75" customHeight="1">
       <c r="N49" s="53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="14:14" ht="15.75" customHeight="1">
       <c r="N50" s="53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="14:14" ht="15.75" customHeight="1">
       <c r="N51" s="53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="14:14" ht="15.75" customHeight="1">
       <c r="N52" s="53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="53" spans="14:14" ht="15.75" customHeight="1">

</xml_diff>